<commit_message>
Objective fct and constraints added
base model fully included
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESchr\workspace\uni\ATIS3\Single_Project\ATIES3_single_project_ES\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CA5CE2-F374-4A57-8440-AC2F49DC938F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9441BF-CD55-4564-A7B6-B6F2E6603874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="4" xr2:uid="{F41D6B2C-A29F-4016-AF80-C7BE5C33C0CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="3" xr2:uid="{F41D6B2C-A29F-4016-AF80-C7BE5C33C0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="bilateral_contract_data" sheetId="1" r:id="rId1"/>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Contract</t>
   </si>
   <si>
-    <t>Usage</t>
-  </si>
-  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>min_power</t>
   </si>
   <si>
-    <t>1.2.3.4</t>
-  </si>
-  <si>
     <t>w1</t>
   </si>
   <si>
@@ -110,12 +104,6 @@
     <t>k1</t>
   </si>
   <si>
-    <t xml:space="preserve">k2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">k3 </t>
-  </si>
-  <si>
     <t>k4</t>
   </si>
   <si>
@@ -207,6 +195,12 @@
   </si>
   <si>
     <t>q15</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>k3</t>
   </si>
 </sst>
 </file>
@@ -565,133 +559,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326D2C6A-7C1E-476A-9A89-D087E262AE4F}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" t="s">
+        <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>48.5</v>
+      </c>
+      <c r="G2">
+        <v>75</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>75</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>49.5</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>51</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>48.5</v>
-      </c>
-      <c r="D2">
-        <v>75</v>
-      </c>
-      <c r="E2">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>49</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>50</v>
       </c>
-      <c r="D3">
-        <v>75</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>49.5</v>
-      </c>
-      <c r="D4">
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>51</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>49</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-      <c r="E6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-      <c r="E7">
+      <c r="H7">
         <v>20</v>
       </c>
     </row>
@@ -706,31 +763,31 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -762,24 +819,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>44</v>
@@ -796,7 +853,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>44</v>
@@ -813,7 +870,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>44</v>
@@ -830,7 +887,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>44</v>
@@ -847,7 +904,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>44</v>
@@ -864,7 +921,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>44</v>
@@ -881,7 +938,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>44</v>
@@ -898,7 +955,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>44</v>
@@ -915,7 +972,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -932,7 +989,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -949,7 +1006,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -966,7 +1023,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -983,7 +1040,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>50</v>
@@ -1000,7 +1057,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>50</v>
@@ -1017,7 +1074,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>50</v>
@@ -1034,7 +1091,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -1059,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899502C1-75FF-49AD-AF2D-93914E598563}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,24 +1127,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1104,7 +1161,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1121,7 +1178,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1138,7 +1195,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1155,7 +1212,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1172,7 +1229,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1189,7 +1246,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1206,7 +1263,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1223,7 +1280,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1240,7 +1297,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1257,7 +1314,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1274,7 +1331,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1291,7 +1348,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1308,7 +1365,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1325,7 +1382,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1350,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4D9919-2431-4026-8FD6-F5920B77E3EE}">
   <dimension ref="A1:B289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
@@ -1358,15 +1415,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1374,7 +1431,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1382,7 +1439,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1390,7 +1447,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1398,7 +1455,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1406,7 +1463,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1414,7 +1471,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1422,7 +1479,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1430,7 +1487,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1438,7 +1495,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1446,7 +1503,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1454,7 +1511,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1462,7 +1519,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1470,7 +1527,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1478,7 +1535,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>0</v>

</xml_diff>

<commit_message>
Customer purchase error solved
PV scenarios included
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESchr\workspace\uni\ATIS3\Single_Project\ATIES3_single_project_ES\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6B968C-64D1-47F2-BF75-CBE20D542E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2815EDE9-775D-4D2C-BD38-1EB77D041AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="4" xr2:uid="{F41D6B2C-A29F-4016-AF80-C7BE5C33C0CD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
   <si>
     <t>Contract</t>
   </si>
@@ -150,12 +150,6 @@
   </si>
   <si>
     <t>k3</t>
-  </si>
-  <si>
-    <t>period</t>
-  </si>
-  <si>
-    <t>pv_power</t>
   </si>
 </sst>
 </file>
@@ -517,7 +511,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +761,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="E17" sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1066,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,52 +1354,301 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4D9919-2431-4026-8FD6-F5920B77E3EE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B3">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>47</v>
+      </c>
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>44</v>
+      </c>
+      <c r="D6">
+        <v>42</v>
+      </c>
+      <c r="E6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B7">
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <v>44</v>
+      </c>
+      <c r="D7">
+        <v>42</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>44</v>
+      </c>
+      <c r="D8">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>52</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>51</v>
+      </c>
+      <c r="E12">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>52</v>
+      </c>
+      <c r="D13">
+        <v>51</v>
+      </c>
+      <c r="E13">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>47</v>
+      </c>
+      <c r="E14">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>48</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>48</v>
+      </c>
+      <c r="E17">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>